<commit_message>
update independent validation plots
</commit_message>
<xml_diff>
--- a/inputs/vars_DV_2022ed_ARCHIVED.xlsx
+++ b/inputs/vars_DV_2022ed_ARCHIVED.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ConsVision_DevVulnModel\inputs\vars\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ConsVision_DevVulnModel\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="54675" yWindow="0" windowWidth="18060" windowHeight="10005"/>
+    <workbookView xWindow="56325" yWindow="0" windowWidth="18060" windowHeight="10005"/>
   </bookViews>
   <sheets>
     <sheet name="vars_20210907" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="224">
   <si>
     <t>raster_basename</t>
   </si>
@@ -686,9 +686,6 @@
   </si>
   <si>
     <t>F:/David/projects/vulnerability_model/vars/nlcd_based/nlcdv19_variables.gdb/lc_cost_2006</t>
-  </si>
-  <si>
-    <t>did not use</t>
   </si>
   <si>
     <t>did not use as a variable. Instead using conslands as a post-model adjustement</t>
@@ -1146,7 +1143,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1971,7 +1968,7 @@
         <v>128</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K23" s="12" t="s">
         <v>143</v>
@@ -2005,9 +2002,7 @@
       <c r="I24" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>222</v>
-      </c>
+      <c r="J24" s="14"/>
       <c r="K24" s="12" t="s">
         <v>171</v>
       </c>
@@ -2040,9 +2035,7 @@
       <c r="I25" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="J25" s="14" t="s">
-        <v>222</v>
-      </c>
+      <c r="J25" s="14"/>
       <c r="K25" s="12" t="s">
         <v>172</v>
       </c>
@@ -2959,7 +2952,7 @@
         <v>141</v>
       </c>
       <c r="J49" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K49" s="12" t="s">
         <v>165</v>
@@ -2994,7 +2987,7 @@
         <v>105</v>
       </c>
       <c r="J50" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K50" s="12" t="s">
         <v>168</v>
@@ -3045,7 +3038,7 @@
         <v>111</v>
       </c>
       <c r="J51" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K51" s="12" t="s">
         <v>170</v>
@@ -3096,7 +3089,7 @@
         <v>99</v>
       </c>
       <c r="J52" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K52" s="12" t="s">
         <v>166</v>

</xml_diff>

<commit_message>
add script overview to README
</commit_message>
<xml_diff>
--- a/inputs/vars_DV_2022ed_ARCHIVED.xlsx
+++ b/inputs/vars_DV_2022ed_ARCHIVED.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ConsVision_DevVulnModel\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\ConsVision_DevVulnModel\inputs\vars\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="56325" yWindow="0" windowWidth="18060" windowHeight="10005"/>
+    <workbookView xWindow="1545" yWindow="0" windowWidth="27255" windowHeight="12885"/>
   </bookViews>
   <sheets>
-    <sheet name="vars_20210907" sheetId="1" r:id="rId1"/>
+    <sheet name="vars" sheetId="1" r:id="rId1"/>
     <sheet name="attr_desc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="225">
   <si>
     <t>raster_basename</t>
   </si>
@@ -688,10 +688,13 @@
     <t>F:/David/projects/vulnerability_model/vars/nlcd_based/nlcdv19_variables.gdb/lc_cost_2006</t>
   </si>
   <si>
-    <t>did not use as a variable. Instead using conslands as a post-model adjustement</t>
+    <t>did not use</t>
   </si>
   <si>
     <t>redundant; not using</t>
+  </si>
+  <si>
+    <t>did not use as a variable. Instead using conslands (BMI-only) as a post-model adjustement</t>
   </si>
 </sst>
 </file>
@@ -1142,19 +1145,20 @@
   <dimension ref="A1:AA1009"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.25" customWidth="1"/>
     <col min="2" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="8" customWidth="1"/>
-    <col min="4" max="5" width="13.125" customWidth="1"/>
-    <col min="6" max="6" width="10.625" customWidth="1"/>
-    <col min="7" max="7" width="8.625" customWidth="1"/>
-    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="3" max="3" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.75" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.375" style="19" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="80.375" bestFit="1" customWidth="1"/>
@@ -1196,146 +1200,144 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>17</v>
+        <v>64</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>17</v>
+        <v>65</v>
       </c>
       <c r="C2" s="12">
         <v>1</v>
       </c>
       <c r="D2" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="13">
         <v>0</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="G2" s="12">
         <v>1</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>138</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="J2" s="14"/>
       <c r="K2" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
       </c>
       <c r="D3" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="G3" s="12">
         <v>1</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="J3" s="14"/>
       <c r="K3" s="12" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="C4" s="12">
         <v>1</v>
       </c>
       <c r="D4" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="G4" s="12">
         <v>1</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="I4" s="17" t="s">
-        <v>29</v>
+        <v>79</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>41</v>
+        <v>81</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
       <c r="D5" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="13">
         <v>0</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G5" s="12">
         <v>100</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>42</v>
+        <v>82</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="12" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
@@ -1347,28 +1349,30 @@
         <v>0</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G6" s="12">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="14"/>
+        <v>19</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>138</v>
+      </c>
       <c r="K6" s="12" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>135</v>
+        <v>23</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C7" s="12">
         <v>1</v>
@@ -1377,31 +1381,31 @@
         <v>0</v>
       </c>
       <c r="E7" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G7" s="12">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="12" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>217</v>
+        <v>28</v>
       </c>
       <c r="C8" s="12">
         <v>1</v>
@@ -1410,31 +1414,31 @@
         <v>0</v>
       </c>
       <c r="E8" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G8" s="12">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>199</v>
+        <v>29</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="C9" s="12">
         <v>1</v>
@@ -1449,25 +1453,25 @@
         <v>31</v>
       </c>
       <c r="G9" s="12">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="H9" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>198</v>
+        <v>42</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="12" t="s">
-        <v>204</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>195</v>
+        <v>132</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>212</v>
+        <v>45</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -1482,17 +1486,17 @@
         <v>31</v>
       </c>
       <c r="G10" s="12">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>197</v>
+        <v>46</v>
       </c>
       <c r="J10" s="14"/>
       <c r="K10" s="12" t="s">
-        <v>202</v>
+        <v>150</v>
       </c>
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
@@ -1513,10 +1517,10 @@
     </row>
     <row r="11" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>193</v>
+        <v>135</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>211</v>
+        <v>51</v>
       </c>
       <c r="C11" s="12">
         <v>1</v>
@@ -1531,17 +1535,17 @@
         <v>31</v>
       </c>
       <c r="G11" s="12">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>200</v>
+        <v>52</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="12" t="s">
-        <v>201</v>
+        <v>153</v>
       </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
@@ -1560,12 +1564,12 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
     </row>
-    <row r="12" spans="1:27" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>62</v>
+        <v>196</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>62</v>
+        <v>217</v>
       </c>
       <c r="C12" s="12">
         <v>1</v>
@@ -1577,20 +1581,20 @@
         <v>0</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="G12" s="12">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="J12" s="15"/>
+        <v>199</v>
+      </c>
+      <c r="J12" s="14"/>
       <c r="K12" s="12" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -1609,117 +1613,117 @@
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
     </row>
-    <row r="13" spans="1:27" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
-        <v>64</v>
+        <v>194</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>65</v>
+        <v>218</v>
       </c>
       <c r="C13" s="12">
         <v>1</v>
       </c>
       <c r="D13" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" s="13">
         <v>0</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="G13" s="12">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>68</v>
+        <v>198</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>70</v>
+        <v>212</v>
       </c>
       <c r="C14" s="12">
         <v>1</v>
       </c>
       <c r="D14" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="13">
         <v>0</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="G14" s="12">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>72</v>
+        <v>197</v>
       </c>
       <c r="J14" s="14"/>
       <c r="K14" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="12" t="s">
-        <v>78</v>
+        <v>193</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>78</v>
+        <v>211</v>
       </c>
       <c r="C15" s="12">
         <v>1</v>
       </c>
       <c r="D15" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="13">
         <v>0</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="G15" s="12">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>79</v>
+        <v>200</v>
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="12" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" s="8" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C16" s="12">
         <v>1</v>
       </c>
       <c r="D16" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="13">
         <v>0</v>
@@ -1728,17 +1732,17 @@
         <v>12</v>
       </c>
       <c r="G16" s="12">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="J16" s="14"/>
+        <v>220</v>
+      </c>
+      <c r="J16" s="15"/>
       <c r="K16" s="12" t="s">
-        <v>160</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:27" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1939,270 +1943,274 @@
         <v>169</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
-        <v>126</v>
+        <v>205</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>127</v>
+        <v>205</v>
       </c>
       <c r="C23" s="12">
         <v>0</v>
       </c>
       <c r="D23" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="13">
         <v>0</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G23" s="12">
         <v>1</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>222</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="J23" s="14"/>
       <c r="K23" s="12" t="s">
-        <v>143</v>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" s="12" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>11</v>
+        <v>206</v>
       </c>
       <c r="C24" s="12">
         <v>0</v>
       </c>
       <c r="D24" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="13">
         <v>0</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G24" s="12">
         <v>1</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>14</v>
+        <v>219</v>
       </c>
       <c r="J24" s="14"/>
       <c r="K24" s="12" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="12" t="s">
-        <v>15</v>
+        <v>213</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>15</v>
+        <v>214</v>
       </c>
       <c r="C25" s="12">
         <v>0</v>
       </c>
       <c r="D25" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="13">
         <v>0</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G25" s="12">
         <v>1</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>16</v>
+        <v>215</v>
       </c>
       <c r="J25" s="14"/>
       <c r="K25" s="12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="12" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="12">
+        <v>73</v>
+      </c>
+      <c r="C26" s="13">
         <v>0</v>
       </c>
       <c r="D26" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="G26" s="12">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="J26" s="14"/>
       <c r="K26" s="12" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="12">
+        <v>76</v>
+      </c>
+      <c r="C27" s="13">
         <v>0</v>
       </c>
       <c r="D27" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="G27" s="12">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="J27" s="14"/>
       <c r="K27" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
-        <v>205</v>
+        <v>126</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>205</v>
+        <v>127</v>
       </c>
       <c r="C28" s="12">
         <v>0</v>
       </c>
       <c r="D28" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="13">
         <v>0</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G28" s="12">
         <v>1</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="J28" s="14"/>
+        <v>128</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>224</v>
+      </c>
       <c r="K28" s="12" t="s">
-        <v>209</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:27" s="8" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="12" t="s">
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>206</v>
+        <v>11</v>
       </c>
       <c r="C29" s="12">
         <v>0</v>
       </c>
       <c r="D29" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" s="13">
         <v>0</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G29" s="12">
         <v>1</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>219</v>
-      </c>
-      <c r="J29" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>222</v>
+      </c>
       <c r="K29" s="12" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" s="8" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>213</v>
+        <v>15</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>214</v>
+        <v>15</v>
       </c>
       <c r="C30" s="12">
         <v>0</v>
       </c>
       <c r="D30" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="13">
         <v>0</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G30" s="12">
         <v>1</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>207</v>
+        <v>13</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="J30" s="14"/>
+        <v>16</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>222</v>
+      </c>
       <c r="K30" s="12" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
@@ -2223,10 +2231,10 @@
     </row>
     <row r="31" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>131</v>
+        <v>20</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C31" s="12">
         <v>0</v>
@@ -2235,23 +2243,23 @@
         <v>0</v>
       </c>
       <c r="E31" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G31" s="12">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="J31" s="14"/>
       <c r="K31" s="12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
@@ -2272,10 +2280,10 @@
     </row>
     <row r="32" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="12" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C32" s="12">
         <v>0</v>
@@ -2284,31 +2292,31 @@
         <v>0</v>
       </c>
       <c r="E32" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="G32" s="12">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="J32" s="14"/>
       <c r="K32" s="12" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C33" s="12">
         <v>0</v>
@@ -2329,19 +2337,19 @@
         <v>56</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J33" s="14"/>
       <c r="K33" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C34" s="12">
         <v>0</v>
@@ -2362,19 +2370,19 @@
         <v>56</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A35" s="12" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C35" s="12">
         <v>0</v>
@@ -2389,27 +2397,25 @@
         <v>31</v>
       </c>
       <c r="G35" s="12">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H35" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="J35" s="14" t="s">
-        <v>129</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="J35" s="14"/>
       <c r="K35" s="12" t="s">
-        <v>173</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C36" s="12">
         <v>0</v>
@@ -2424,19 +2430,17 @@
         <v>31</v>
       </c>
       <c r="G36" s="12">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="H36" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J36" s="14" t="s">
-        <v>129</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="J36" s="14"/>
       <c r="K36" s="12" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="L36" s="7"/>
       <c r="M36" s="7"/>
@@ -2457,10 +2461,10 @@
     </row>
     <row r="37" spans="1:27" s="8" customFormat="1" ht="39" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C37" s="12">
         <v>0</v>
@@ -2481,13 +2485,13 @@
         <v>56</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>129</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L37" s="7"/>
       <c r="M37" s="7"/>
@@ -2508,10 +2512,10 @@
     </row>
     <row r="38" spans="1:27" s="8" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C38" s="12">
         <v>0</v>
@@ -2532,21 +2536,21 @@
         <v>56</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>129</v>
       </c>
       <c r="K38" s="12" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C39" s="12">
         <v>0</v>
@@ -2567,21 +2571,21 @@
         <v>56</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>129</v>
       </c>
       <c r="K39" s="12" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="12" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C40" s="12">
         <v>0</v>
@@ -2593,28 +2597,30 @@
         <v>0</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G40" s="12">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J40" s="14"/>
+        <v>38</v>
+      </c>
+      <c r="J40" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="K40" s="12" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:27" ht="39" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>124</v>
+        <v>39</v>
       </c>
       <c r="C41" s="12">
         <v>0</v>
@@ -2629,17 +2635,19 @@
         <v>31</v>
       </c>
       <c r="G41" s="12">
-        <v>10000</v>
+        <v>100</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="J41" s="14"/>
+        <v>40</v>
+      </c>
+      <c r="J41" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="K41" s="12" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="L41" s="2"/>
       <c r="M41" s="2"/>
@@ -2660,12 +2668,12 @@
     </row>
     <row r="42" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="13">
+        <v>58</v>
+      </c>
+      <c r="C42" s="12">
         <v>0</v>
       </c>
       <c r="D42" s="13">
@@ -2684,13 +2692,11 @@
         <v>56</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="J42" s="14" t="s">
-        <v>129</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="J42" s="14"/>
       <c r="K42" s="12" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
@@ -2709,12 +2715,12 @@
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
     </row>
-    <row r="43" spans="1:27" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="39" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>60</v>
+        <v>124</v>
       </c>
       <c r="C43" s="12">
         <v>0</v>
@@ -2726,20 +2732,20 @@
         <v>0</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G43" s="12">
-        <v>1</v>
+        <v>10000</v>
       </c>
       <c r="H43" s="12" t="s">
         <v>56</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="J43" s="15"/>
+        <v>125</v>
+      </c>
+      <c r="J43" s="14"/>
       <c r="K43" s="12" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
@@ -2758,70 +2764,72 @@
       <c r="Z43" s="2"/>
       <c r="AA43" s="2"/>
     </row>
-    <row r="44" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="12" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C44" s="13">
         <v>0</v>
       </c>
       <c r="D44" s="13">
+        <v>0</v>
+      </c>
+      <c r="E44" s="13">
+        <v>0</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="12">
         <v>1</v>
       </c>
-      <c r="E44" s="13">
-        <v>0</v>
-      </c>
-      <c r="F44" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G44" s="12">
-        <v>1000</v>
-      </c>
       <c r="H44" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="J44" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="J44" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="K44" s="12" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" ht="14.25" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" s="12" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C45" s="13">
+        <v>60</v>
+      </c>
+      <c r="C45" s="12">
         <v>0</v>
       </c>
       <c r="D45" s="13">
+        <v>0</v>
+      </c>
+      <c r="E45" s="13">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="12">
         <v>1</v>
       </c>
-      <c r="E45" s="13">
-        <v>0</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G45" s="12">
-        <v>1000</v>
-      </c>
       <c r="H45" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="J45" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="J45" s="15"/>
       <c r="K45" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">

</xml_diff>